<commit_message>
Atualizações na documentação: cronograma do sprint 1.
</commit_message>
<xml_diff>
--- a/docs/Project Docs/MSL_CP_CronogramaDoProjeto.xlsx
+++ b/docs/Project Docs/MSL_CP_CronogramaDoProjeto.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="98">
   <si>
     <t>Real</t>
   </si>
@@ -393,12 +393,18 @@
   <si>
     <t>Criar página (view laravel) para criar/logar conta. Criar uma página home incial para ser a próxima página após o login. Nessa página home deve haver em algum lugar um menu com opções de deslogar e excluir a conta. Nos formulários para logar, criar conta, excluir e sair, a ação do form html deve ser um POST no respectivo endpoint. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
   </si>
+  <si>
+    <t>Testes de aceitação</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -566,8 +572,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -633,8 +647,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -723,6 +749,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -749,7 +790,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -930,6 +971,21 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -948,26 +1004,35 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1930,14 +1995,14 @@
       <c r="AG1" s="13"/>
     </row>
     <row r="2" spans="2:213" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
       <c r="H2" s="50" t="s">
         <v>3</v>
       </c>
@@ -1967,12 +2032,12 @@
       <c r="AG2" s="6"/>
     </row>
     <row r="3" spans="2:213" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -1992,12 +2057,12 @@
       <c r="AG3" s="6"/>
     </row>
     <row r="4" spans="2:213" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
       <c r="H4" s="50" t="s">
         <v>7</v>
       </c>
@@ -2035,12 +2100,12 @@
       <c r="AT4" s="5"/>
     </row>
     <row r="5" spans="2:213" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -12729,11 +12794,11 @@
       <c r="AG55" s="13"/>
     </row>
     <row r="56" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="56" t="s">
+      <c r="B56" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="56"/>
-      <c r="D56" s="56"/>
+      <c r="C56" s="61"/>
+      <c r="D56" s="61"/>
       <c r="E56" s="13"/>
       <c r="F56" s="29"/>
       <c r="G56" s="13"/>
@@ -12765,12 +12830,12 @@
       <c r="AG56" s="13"/>
     </row>
     <row r="57" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="57">
+      <c r="B57" s="62">
         <f>'Cronograma + Diagrama de Gantt'!$F$7</f>
         <v>5.128205128205128E-2</v>
       </c>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
       <c r="E57" s="13"/>
       <c r="F57" s="29"/>
       <c r="G57" s="13"/>
@@ -12802,9 +12867,9 @@
       <c r="AG57" s="13"/>
     </row>
     <row r="58" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="57"/>
-      <c r="C58" s="57"/>
-      <c r="D58" s="57"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
       <c r="E58" s="13"/>
       <c r="F58" s="29"/>
       <c r="G58" s="13"/>
@@ -12836,9 +12901,9 @@
       <c r="AG58" s="13"/>
     </row>
     <row r="59" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="57"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="57"/>
+      <c r="B59" s="62"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="62"/>
       <c r="E59" s="13"/>
       <c r="F59" s="29"/>
       <c r="G59" s="13"/>
@@ -12870,9 +12935,9 @@
       <c r="AG59" s="13"/>
     </row>
     <row r="60" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="57"/>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
+      <c r="B60" s="62"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="62"/>
       <c r="E60" s="13"/>
       <c r="F60" s="29"/>
       <c r="G60" s="13"/>
@@ -34196,20 +34261,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.875" customWidth="1"/>
     <col min="2" max="2" width="71.625" customWidth="1"/>
-    <col min="3" max="3" width="15.125" style="65" customWidth="1"/>
-    <col min="4" max="4" width="11" style="65" customWidth="1"/>
-    <col min="5" max="5" width="10.375" style="65" customWidth="1"/>
-    <col min="6" max="6" width="11.25" style="65" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="59" customWidth="1"/>
+    <col min="4" max="4" width="11" style="59" customWidth="1"/>
+    <col min="5" max="5" width="10.375" style="59" customWidth="1"/>
+    <col min="6" max="6" width="11.25" style="59" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -34219,83 +34284,83 @@
       <c r="B1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="62"/>
-      <c r="F1" s="63"/>
+      <c r="D1" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="57"/>
+      <c r="F1" s="58"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
     </row>
     <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="59"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A5" s="64"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="72" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="64" t="s">
+      <c r="F6" s="72" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="69" t="s">
         <v>86</v>
       </c>
       <c r="D7" s="66">
@@ -34304,144 +34369,164 @@
       <c r="E7" s="66">
         <v>42504</v>
       </c>
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="69" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="69" t="s">
         <v>85</v>
       </c>
       <c r="D8" s="66">
         <v>42503</v>
       </c>
       <c r="E8" s="66">
-        <v>42503</v>
-      </c>
-      <c r="F8" s="65" t="s">
+        <v>42504</v>
+      </c>
+      <c r="F8" s="69" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="66">
-        <v>42503</v>
-      </c>
-      <c r="E9" s="66">
-        <v>42504</v>
-      </c>
-      <c r="F9" s="65" t="s">
+      <c r="D9" s="68">
+        <v>42505</v>
+      </c>
+      <c r="E9" s="68">
+        <v>42506</v>
+      </c>
+      <c r="F9" s="70" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="66">
-        <v>42503</v>
-      </c>
-      <c r="E10" s="66">
-        <v>42504</v>
-      </c>
-      <c r="F10" s="65" t="s">
+      <c r="D10" s="68">
+        <v>42505</v>
+      </c>
+      <c r="E10" s="68">
+        <v>42506</v>
+      </c>
+      <c r="F10" s="70" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="66">
-        <v>42503</v>
-      </c>
-      <c r="E11" s="66">
-        <v>42504</v>
-      </c>
-      <c r="F11" s="65" t="s">
+      <c r="D11" s="68">
+        <v>42507</v>
+      </c>
+      <c r="E11" s="68">
+        <v>42508</v>
+      </c>
+      <c r="F11" s="70" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="68">
+        <v>42509</v>
+      </c>
+      <c r="E12" s="68">
+        <v>42509</v>
+      </c>
+      <c r="F12" s="70" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C13" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="66">
-        <v>42504</v>
-      </c>
-      <c r="E12" s="66">
-        <v>42504</v>
-      </c>
-      <c r="F12" s="65" t="s">
+      <c r="D13" s="68">
+        <v>42509</v>
+      </c>
+      <c r="E13" s="68">
+        <v>42509</v>
+      </c>
+      <c r="F13" s="70" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="74" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B14" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C14" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="66">
-        <v>42504</v>
-      </c>
-      <c r="E13" s="66">
-        <v>42504</v>
-      </c>
-      <c r="F13" s="65" t="s">
+      <c r="D14" s="68">
+        <v>42509</v>
+      </c>
+      <c r="E14" s="68">
+        <v>42509</v>
+      </c>
+      <c r="F14" s="70" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="60"/>
-    </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="60"/>
+      <c r="B15" s="55"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="60"/>
+      <c r="B16" s="55"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="60"/>
+      <c r="B17" s="55"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="60"/>
+      <c r="B18" s="55"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Atualizações na documentação: Sprint planning da Sprint 2.
</commit_message>
<xml_diff>
--- a/docs/Project Docs/MSL_CP_CronogramaDoProjeto.xlsx
+++ b/docs/Project Docs/MSL_CP_CronogramaDoProjeto.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma + Diagrama de Gantt" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 2" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cronograma + Diagrama de Gantt'!$B$6:$L$6</definedName>
@@ -26,7 +27,7 @@
     <definedName name="Real">(PeriodoInReal*('Cronograma + Diagrama de Gantt'!$H1&gt;0))*PeriodoInPlanejado</definedName>
     <definedName name="RealPosterior">PeriodoInReal*('Cronograma + Diagrama de Gantt'!$H1&gt;0)</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="106">
   <si>
     <t>Real</t>
   </si>
@@ -370,9 +371,6 @@
     <t>Michel Berigo</t>
   </si>
   <si>
-    <t>Não inciada</t>
-  </si>
-  <si>
     <t>Conectar a aplicação laravel criada com o banco de dados (dados do banco estarão disponíveis no documento de senhas). Então criar os models referentes as tabelas criadas no banco de dados. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
   </si>
   <si>
@@ -400,16 +398,51 @@
     <t>1.1</t>
   </si>
   <si>
-    <t>Entregue</t>
+    <t>Data Entrega</t>
   </si>
   <si>
-    <t>Data Entrega</t>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>Concluída</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Projeto My Study Life
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="36"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sprint 2</t>
+    </r>
+  </si>
+  <si>
+    <t>Criar endpoints/views na aplicação para um usuário alterar a senha, email e seu nome de usuário, não são permitidos usuários iguais. Endpoints devem ser documentados no documento de endpoints. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
+  </si>
+  <si>
+    <t>Criar página (view laravel) para alterar as informaçes de usuarios tais como nome de usuario, email e senha. Criar uma página que sera acessada atraves do menu de usuario. Nessa página deve haver uma confirmaçao onde sera solicitada a senha atual do usuario para que sejam efetuadas as alteraçoes no cadastro. No formulário, a ação do form html deve ser um POST nos respectivos endpoints. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
+  </si>
+  <si>
+    <t>Em espera</t>
+  </si>
+  <si>
+    <t>Criar endpoints/views na aplicação para um usuário recuperar a senha, um e-mail deve ser enviado para o usuário que terá que redefinir sua senha. Endpoints devem ser documentados no documento de endpoints. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
+  </si>
+  <si>
+    <t>Modelar e criar conceitos do banco de dados de ano letivo, semestre, disciplina, atividades e provas, considerando suas respectivas ligações no banco de dados. Os scripts usados para criar o banco devem ser inseridos por meio de documento no diretório de documentos do código. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1022,6 +1055,9 @@
     <xf numFmtId="14" fontId="0" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1040,9 +1076,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Activity" xfId="2"/>
@@ -1055,7 +1088,37 @@
     <cellStyle name="Project Headers" xfId="4"/>
     <cellStyle name="Título 1" xfId="1" builtinId="16" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF004080"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1936,8 +1999,8 @@
   </sheetPr>
   <dimension ref="B1:HE701"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -2004,14 +2067,14 @@
       <c r="AG1" s="13"/>
     </row>
     <row r="2" spans="2:213" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
       <c r="H2" s="50" t="s">
         <v>3</v>
       </c>
@@ -2041,12 +2104,12 @@
       <c r="AG2" s="6"/>
     </row>
     <row r="3" spans="2:213" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2066,12 +2129,12 @@
       <c r="AG3" s="6"/>
     </row>
     <row r="4" spans="2:213" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
       <c r="H4" s="50" t="s">
         <v>7</v>
       </c>
@@ -2109,12 +2172,12 @@
       <c r="AT4" s="5"/>
     </row>
     <row r="5" spans="2:213" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -2983,7 +3046,7 @@
       </c>
       <c r="E7" s="43">
         <f>(J7-H7)+1</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F7" s="36">
         <f>AVERAGE($F$9:$F$48)</f>
@@ -3003,7 +3066,7 @@
       </c>
       <c r="J7" s="37">
         <f>LARGE($J$8:$J$47,1)</f>
-        <v>42503</v>
+        <v>42510</v>
       </c>
       <c r="K7" s="37"/>
       <c r="L7" s="38"/>
@@ -3052,8 +3115,7 @@
         <v>42496</v>
       </c>
       <c r="I8" s="27">
-        <f>(G8+D8)-1</f>
-        <v>42492</v>
+        <v>42496</v>
       </c>
       <c r="J8" s="27">
         <f>(H8+E8)-1</f>
@@ -3288,7 +3350,7 @@
         <v>42496</v>
       </c>
       <c r="H9" s="10">
-        <v>42499</v>
+        <v>42496</v>
       </c>
       <c r="I9" s="27">
         <f t="shared" ref="I9:I10" si="142">(G9+D9)-1</f>
@@ -3296,7 +3358,7 @@
       </c>
       <c r="J9" s="27">
         <f t="shared" ref="J9:J47" si="143">(H9+E9)-1</f>
-        <v>42502</v>
+        <v>42499</v>
       </c>
       <c r="K9" s="27" t="str">
         <f t="shared" ca="1" si="141"/>
@@ -3534,8 +3596,7 @@
         <v>42503</v>
       </c>
       <c r="J10" s="27">
-        <f t="shared" si="143"/>
-        <v>42503</v>
+        <v>42510</v>
       </c>
       <c r="K10" s="27" t="str">
         <f t="shared" ca="1" si="141"/>
@@ -3773,12 +3834,10 @@
         <v>42504</v>
       </c>
       <c r="J11" s="27">
-        <f t="shared" ref="J11:J13" si="144">(H11+E11)-1</f>
-        <v>42503</v>
-      </c>
-      <c r="K11" s="27" t="str">
-        <f t="shared" ref="K11:K13" ca="1" si="145">IF(F11=1,"Concluído",IF(AND(J11&lt;TODAY(),F11&lt;1),"Em atraso","Em andamento"))</f>
-        <v>Em atraso</v>
+        <v>42510</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="L11" s="41" t="s">
         <v>34</v>
@@ -4012,12 +4071,10 @@
         <v>42504</v>
       </c>
       <c r="J12" s="27">
-        <f t="shared" si="144"/>
-        <v>42503</v>
-      </c>
-      <c r="K12" s="27" t="str">
-        <f t="shared" ca="1" si="145"/>
-        <v>Em atraso</v>
+        <v>42510</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="L12" s="41" t="s">
         <v>34</v>
@@ -4251,12 +4308,10 @@
         <v>42504</v>
       </c>
       <c r="J13" s="27">
-        <f t="shared" si="144"/>
-        <v>42503</v>
-      </c>
-      <c r="K13" s="27" t="str">
-        <f t="shared" ca="1" si="145"/>
-        <v>Em atraso</v>
+        <v>42510</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="L13" s="41" t="s">
         <v>34</v>
@@ -4490,12 +4545,10 @@
         <v>42504</v>
       </c>
       <c r="J14" s="27">
-        <f t="shared" si="143"/>
-        <v>42503</v>
-      </c>
-      <c r="K14" s="27" t="str">
-        <f t="shared" ca="1" si="141"/>
-        <v>Em atraso</v>
+        <v>42510</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="L14" s="41" t="s">
         <v>34</v>
@@ -4719,7 +4772,7 @@
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="27">
-        <f t="shared" ref="I15:I46" si="146">(G15+D15)-1</f>
+        <f t="shared" ref="I15:I46" si="144">(G15+D15)-1</f>
         <v>42504</v>
       </c>
       <c r="J15" s="27">
@@ -4952,7 +5005,7 @@
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J16" s="27">
@@ -5185,7 +5238,7 @@
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J17" s="27">
@@ -5418,15 +5471,15 @@
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J18" s="27">
-        <f t="shared" ref="J18:J46" si="147">(H18+E18)-1</f>
+        <f t="shared" ref="J18:J46" si="145">(H18+E18)-1</f>
         <v>-1</v>
       </c>
       <c r="K18" s="27" t="str">
-        <f t="shared" ref="K18:K46" ca="1" si="148">IF(F18=1,"Concluído",IF(AND(J18&lt;TODAY(),F18&lt;1),"Em atraso","Em andamento"))</f>
+        <f t="shared" ref="K18:K46" ca="1" si="146">IF(F18=1,"Concluído",IF(AND(J18&lt;TODAY(),F18&lt;1),"Em atraso","Em andamento"))</f>
         <v>Em atraso</v>
       </c>
       <c r="L18" s="41" t="s">
@@ -5651,15 +5704,15 @@
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J19" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K19" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L19" s="41" t="s">
@@ -5884,15 +5937,15 @@
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J20" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K20" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L20" s="41" t="s">
@@ -6117,15 +6170,15 @@
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J21" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K21" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L21" s="41" t="s">
@@ -6350,15 +6403,15 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J22" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K22" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L22" s="41" t="s">
@@ -6583,15 +6636,15 @@
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J23" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K23" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L23" s="41" t="s">
@@ -6816,15 +6869,15 @@
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J24" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K24" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L24" s="41" t="s">
@@ -7049,15 +7102,15 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J25" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K25" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L25" s="41" t="s">
@@ -7282,15 +7335,15 @@
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J26" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K26" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L26" s="41" t="s">
@@ -7515,15 +7568,15 @@
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J27" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K27" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L27" s="41" t="s">
@@ -7748,15 +7801,15 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J28" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K28" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L28" s="41" t="s">
@@ -7981,15 +8034,15 @@
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J29" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K29" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L29" s="41" t="s">
@@ -8214,15 +8267,15 @@
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J30" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K30" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L30" s="41" t="s">
@@ -8447,15 +8500,15 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J31" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K31" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L31" s="41" t="s">
@@ -8680,15 +8733,15 @@
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J32" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K32" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L32" s="41" t="s">
@@ -8913,15 +8966,15 @@
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J33" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K33" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L33" s="41" t="s">
@@ -9146,15 +9199,15 @@
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J34" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K34" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L34" s="41" t="s">
@@ -9379,15 +9432,15 @@
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J35" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K35" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L35" s="41" t="s">
@@ -9612,15 +9665,15 @@
       </c>
       <c r="H36" s="10"/>
       <c r="I36" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J36" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K36" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L36" s="41" t="s">
@@ -9845,15 +9898,15 @@
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J37" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K37" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L37" s="41" t="s">
@@ -10078,15 +10131,15 @@
       </c>
       <c r="H38" s="10"/>
       <c r="I38" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J38" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K38" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L38" s="41" t="s">
@@ -10311,15 +10364,15 @@
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J39" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K39" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L39" s="41" t="s">
@@ -10544,15 +10597,15 @@
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J40" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K40" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L40" s="41" t="s">
@@ -10777,15 +10830,15 @@
       </c>
       <c r="H41" s="10"/>
       <c r="I41" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J41" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K41" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L41" s="41" t="s">
@@ -11010,15 +11063,15 @@
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J42" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K42" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L42" s="41" t="s">
@@ -11243,15 +11296,15 @@
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J43" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K43" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L43" s="41" t="s">
@@ -11476,15 +11529,15 @@
       </c>
       <c r="H44" s="10"/>
       <c r="I44" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J44" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K44" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L44" s="41" t="s">
@@ -11709,15 +11762,15 @@
       </c>
       <c r="H45" s="10"/>
       <c r="I45" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J45" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K45" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L45" s="41" t="s">
@@ -11942,15 +11995,15 @@
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="144"/>
         <v>42504</v>
       </c>
       <c r="J46" s="27">
-        <f t="shared" si="147"/>
+        <f t="shared" si="145"/>
         <v>-1</v>
       </c>
       <c r="K46" s="27" t="str">
-        <f t="shared" ca="1" si="148"/>
+        <f t="shared" ca="1" si="146"/>
         <v>Em atraso</v>
       </c>
       <c r="L46" s="41" t="s">
@@ -12671,11 +12724,11 @@
       <c r="AG55" s="13"/>
     </row>
     <row r="56" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="71" t="s">
+      <c r="B56" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="71"/>
-      <c r="D56" s="71"/>
+      <c r="C56" s="72"/>
+      <c r="D56" s="72"/>
       <c r="E56" s="13"/>
       <c r="F56" s="29"/>
       <c r="G56" s="13"/>
@@ -12707,12 +12760,12 @@
       <c r="AG56" s="13"/>
     </row>
     <row r="57" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="72">
+      <c r="B57" s="73">
         <f>'Cronograma + Diagrama de Gantt'!$F$7</f>
         <v>5.128205128205128E-2</v>
       </c>
-      <c r="C57" s="72"/>
-      <c r="D57" s="72"/>
+      <c r="C57" s="73"/>
+      <c r="D57" s="73"/>
       <c r="E57" s="13"/>
       <c r="F57" s="29"/>
       <c r="G57" s="13"/>
@@ -12744,9 +12797,9 @@
       <c r="AG57" s="13"/>
     </row>
     <row r="58" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="72"/>
-      <c r="C58" s="72"/>
-      <c r="D58" s="72"/>
+      <c r="B58" s="73"/>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
       <c r="E58" s="13"/>
       <c r="F58" s="29"/>
       <c r="G58" s="13"/>
@@ -12778,9 +12831,9 @@
       <c r="AG58" s="13"/>
     </row>
     <row r="59" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="72"/>
-      <c r="C59" s="72"/>
-      <c r="D59" s="72"/>
+      <c r="B59" s="73"/>
+      <c r="C59" s="73"/>
+      <c r="D59" s="73"/>
       <c r="E59" s="13"/>
       <c r="F59" s="29"/>
       <c r="G59" s="13"/>
@@ -12812,9 +12865,9 @@
       <c r="AG59" s="13"/>
     </row>
     <row r="60" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="72"/>
-      <c r="C60" s="72"/>
-      <c r="D60" s="72"/>
+      <c r="B60" s="73"/>
+      <c r="C60" s="73"/>
+      <c r="D60" s="73"/>
       <c r="E60" s="13"/>
       <c r="F60" s="29"/>
       <c r="G60" s="13"/>
@@ -34007,93 +34060,104 @@
     <mergeCell ref="B57:D60"/>
   </mergeCells>
   <conditionalFormatting sqref="C48:BU48">
-    <cfRule type="expression" dxfId="23" priority="385">
+    <cfRule type="expression" dxfId="26" priority="388">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:HE47">
-    <cfRule type="expression" dxfId="22" priority="468">
+    <cfRule type="expression" dxfId="25" priority="471">
       <formula>PorcentagemConcluída</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="469">
+    <cfRule type="expression" dxfId="24" priority="472">
       <formula>PorcentagemConcluídaPosterior</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="470">
+    <cfRule type="expression" dxfId="23" priority="473">
       <formula>Real</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="471">
+    <cfRule type="expression" dxfId="22" priority="474">
       <formula>RealPosterior</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="472">
+    <cfRule type="expression" dxfId="21" priority="475">
       <formula>Plano</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="473">
+    <cfRule type="expression" dxfId="20" priority="476">
       <formula>N$6=$J$4+periodo_selecionado-1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="474">
+    <cfRule type="expression" dxfId="19" priority="477">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="475">
+    <cfRule type="expression" dxfId="18" priority="478">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6:HE6">
-    <cfRule type="expression" dxfId="14" priority="476">
+    <cfRule type="expression" dxfId="17" priority="479">
       <formula>N$6=$J$4+periodo_selecionado-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV48:HE48">
-    <cfRule type="expression" dxfId="13" priority="383">
+    <cfRule type="expression" dxfId="16" priority="386">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K10 K14 K18 K22 K26 K30 K34 K38 K42 K46:K47">
-    <cfRule type="containsText" dxfId="12" priority="376" operator="containsText" text="Em andamento">
+    <cfRule type="containsText" dxfId="15" priority="379" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="377" operator="containsText" text="Em atraso">
+    <cfRule type="containsText" dxfId="14" priority="380" operator="containsText" text="Em atraso">
       <formula>NOT(ISERROR(SEARCH("Em atraso",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="378" operator="containsText" text="Concluído">
+    <cfRule type="containsText" dxfId="13" priority="381" operator="containsText" text="Concluído">
       <formula>NOT(ISERROR(SEARCH("Concluído",K8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="9" priority="375">
+    <cfRule type="expression" dxfId="12" priority="378">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K11 K15 K19 K23 K27 K31 K35 K39 K43">
-    <cfRule type="containsText" dxfId="8" priority="364" operator="containsText" text="Em andamento">
-      <formula>NOT(ISERROR(SEARCH("Em andamento",K11)))</formula>
+  <conditionalFormatting sqref="K15 K19 K23 K27 K31 K35 K39 K43">
+    <cfRule type="containsText" dxfId="11" priority="367" operator="containsText" text="Em andamento">
+      <formula>NOT(ISERROR(SEARCH("Em andamento",K15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="365" operator="containsText" text="Em atraso">
-      <formula>NOT(ISERROR(SEARCH("Em atraso",K11)))</formula>
+    <cfRule type="containsText" dxfId="10" priority="368" operator="containsText" text="Em atraso">
+      <formula>NOT(ISERROR(SEARCH("Em atraso",K15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="366" operator="containsText" text="Concluído">
-      <formula>NOT(ISERROR(SEARCH("Concluído",K11)))</formula>
+    <cfRule type="containsText" dxfId="9" priority="369" operator="containsText" text="Concluído">
+      <formula>NOT(ISERROR(SEARCH("Concluído",K15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12 K16 K20 K24 K28 K32 K36 K40 K44">
-    <cfRule type="containsText" dxfId="5" priority="353" operator="containsText" text="Em andamento">
+    <cfRule type="containsText" dxfId="8" priority="356" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="354" operator="containsText" text="Em atraso">
+    <cfRule type="containsText" dxfId="7" priority="357" operator="containsText" text="Em atraso">
       <formula>NOT(ISERROR(SEARCH("Em atraso",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="355" operator="containsText" text="Concluído">
+    <cfRule type="containsText" dxfId="6" priority="358" operator="containsText" text="Concluído">
       <formula>NOT(ISERROR(SEARCH("Concluído",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13 K17 K21 K25 K29 K33 K37 K41 K45">
-    <cfRule type="containsText" dxfId="2" priority="342" operator="containsText" text="Em andamento">
+    <cfRule type="containsText" dxfId="5" priority="345" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="343" operator="containsText" text="Em atraso">
+    <cfRule type="containsText" dxfId="4" priority="346" operator="containsText" text="Em atraso">
       <formula>NOT(ISERROR(SEARCH("Em atraso",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="344" operator="containsText" text="Concluído">
+    <cfRule type="containsText" dxfId="3" priority="347" operator="containsText" text="Concluído">
       <formula>NOT(ISERROR(SEARCH("Concluído",K13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Em andamento">
+      <formula>NOT(ISERROR(SEARCH("Em andamento",K11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Em atraso">
+      <formula>NOT(ISERROR(SEARCH("Em atraso",K11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Concluído">
+      <formula>NOT(ISERROR(SEARCH("Concluído",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -34140,8 +34204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34166,55 +34230,55 @@
         <v>29</v>
       </c>
       <c r="D1" s="57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E1" s="57"/>
       <c r="F1" s="57"/>
       <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="74" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="A3" s="75"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="74"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="63" t="s">
@@ -34233,7 +34297,7 @@
         <v>72</v>
       </c>
       <c r="F6" s="64" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G6" s="64" t="s">
         <v>73</v>
@@ -34255,11 +34319,11 @@
       <c r="E7" s="69">
         <v>42504</v>
       </c>
-      <c r="F7" s="75">
+      <c r="F7" s="70">
         <v>42506</v>
       </c>
       <c r="G7" s="68" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -34278,11 +34342,314 @@
       <c r="E8" s="69">
         <v>42504</v>
       </c>
-      <c r="F8" s="75">
+      <c r="F8" s="70">
         <v>42505</v>
       </c>
       <c r="G8" s="68" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="69">
+        <v>42505</v>
+      </c>
+      <c r="E9" s="69">
+        <v>42506</v>
+      </c>
+      <c r="F9" s="70">
+        <v>42510</v>
+      </c>
+      <c r="G9" s="68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="69">
+        <v>42505</v>
+      </c>
+      <c r="E10" s="69">
+        <v>42506</v>
+      </c>
+      <c r="F10" s="70">
+        <v>42510</v>
+      </c>
+      <c r="G10" s="68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="69">
+        <v>42507</v>
+      </c>
+      <c r="E11" s="69">
+        <v>42508</v>
+      </c>
+      <c r="F11" s="70">
+        <v>42510</v>
+      </c>
+      <c r="G11" s="68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="66" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="69">
+        <v>42509</v>
+      </c>
+      <c r="E12" s="69">
+        <v>42509</v>
+      </c>
+      <c r="F12" s="70">
+        <v>42510</v>
+      </c>
+      <c r="G12" s="68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="66" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="69">
+        <v>42509</v>
+      </c>
+      <c r="E13" s="69">
+        <v>42509</v>
+      </c>
+      <c r="F13" s="70">
+        <v>42510</v>
+      </c>
+      <c r="G13" s="68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="69">
+        <v>42509</v>
+      </c>
+      <c r="E14" s="69">
+        <v>42509</v>
+      </c>
+      <c r="F14" s="70">
+        <v>42510</v>
+      </c>
+      <c r="G14" s="68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="55"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="55"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="55"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="55"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:G5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D9" activeCellId="5" sqref="D8 E8 F8 F9 E9 D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="71.625" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="59" customWidth="1"/>
+    <col min="4" max="4" width="11" style="59" customWidth="1"/>
+    <col min="5" max="5" width="10.375" style="59" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="59" customWidth="1"/>
+    <col min="7" max="7" width="11.25" style="59" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="58"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+    </row>
+    <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A4" s="75"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="61">
+        <v>42518</v>
+      </c>
+      <c r="E7" s="61">
+        <v>42519</v>
+      </c>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -34290,44 +34657,36 @@
         <v>77</v>
       </c>
       <c r="B9" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="62" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="61">
-        <v>42505</v>
-      </c>
-      <c r="E9" s="61">
-        <v>42506</v>
-      </c>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
       <c r="F9" s="61"/>
       <c r="G9" s="62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
         <v>78</v>
       </c>
       <c r="B10" s="60" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C10" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="61">
-        <v>42505</v>
-      </c>
-      <c r="E10" s="61">
-        <v>42506</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
       <c r="F10" s="61"/>
       <c r="G10" s="62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
         <v>79</v>
       </c>
@@ -34335,17 +34694,17 @@
         <v>95</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D11" s="61">
-        <v>42507</v>
+        <v>42509</v>
       </c>
       <c r="E11" s="61">
-        <v>42508</v>
+        <v>42509</v>
       </c>
       <c r="F11" s="61"/>
       <c r="G11" s="62" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -34353,10 +34712,10 @@
         <v>80</v>
       </c>
       <c r="B12" s="60" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="61">
         <v>42509</v>
@@ -34366,12 +34725,12 @@
       </c>
       <c r="F12" s="61"/>
       <c r="G12" s="62" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="65" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B13" s="60" t="s">
         <v>93</v>
@@ -34387,44 +34746,35 @@
       </c>
       <c r="F13" s="61"/>
       <c r="G13" s="62" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="65" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="60" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="61">
-        <v>42509</v>
-      </c>
-      <c r="E14" s="61">
-        <v>42509</v>
-      </c>
-      <c r="F14" s="61"/>
-      <c r="G14" s="62" t="s">
-        <v>88</v>
-      </c>
+      <c r="B14" s="55"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="55"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16"/>
       <c r="B16" s="55"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17"/>
       <c r="B17" s="55"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18"/>
       <c r="B18" s="55"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="55"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Atualizações na documentação: Cronograma da Sprint 2
</commit_message>
<xml_diff>
--- a/docs/Project Docs/MSL_CP_CronogramaDoProjeto.xlsx
+++ b/docs/Project Docs/MSL_CP_CronogramaDoProjeto.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="121">
   <si>
     <t>Real</t>
   </si>
@@ -424,12 +424,6 @@
     </r>
   </si>
   <si>
-    <t>Criar endpoints/views na aplicação para um usuário alterar a senha, email e seu nome de usuário, não são permitidos usuários iguais. Endpoints devem ser documentados no documento de endpoints. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
-  </si>
-  <si>
-    <t>Criar página (view laravel) para alterar as informaçes de usuarios tais como nome de usuario, email e senha. Criar uma página que sera acessada atraves do menu de usuario. Nessa página deve haver uma confirmaçao onde sera solicitada a senha atual do usuario para que sejam efetuadas as alteraçoes no cadastro. No formulário, a ação do form html deve ser um POST nos respectivos endpoints. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
-  </si>
-  <si>
     <t>Em espera</t>
   </si>
   <si>
@@ -437,6 +431,57 @@
   </si>
   <si>
     <t>Modelar e criar conceitos do banco de dados de ano letivo, semestre, disciplina, atividades e provas, considerando suas respectivas ligações no banco de dados. Os scripts usados para criar o banco devem ser inseridos por meio de documento no diretório de documentos do código. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
+  </si>
+  <si>
+    <t>Criar endpoints na aplicação para um usuário alterar a senha, email e seu nome de usuário, não são permitidos usuários iguais. Endpoints devem ser documentados no documento de endpoints. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
+  </si>
+  <si>
+    <t>Criar endpoints/view na aplicação para criar e associar um horário a uma disciplina. Endpoints devem ser documentados no documento de endpoints. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
+  </si>
+  <si>
+    <t>Criar endpoints/view na aplicação para cadastrar data de provas e trabalhos de uma disciplina. Endpoints devem ser documentados no documento de endpoints. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
+  </si>
+  <si>
+    <t>Criar endpoints/view na aplicação para criar um ano letivo e um novo semestre letivo. Endpoints devem ser documentados no documento de endpoints. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
+  </si>
+  <si>
+    <t>TASK-08</t>
+  </si>
+  <si>
+    <t>TASK-09</t>
+  </si>
+  <si>
+    <t>Criar página (view laravel) para alterar as informaçes de usuarios tais como nome de usuario, email e senha. Criar uma página que sera acessada atraves do menu de usuario. Nessa página deve haver uma confirmaçao onde sera solicitada a senha atual do usuario para que sejam efetuadas as alteraçoes no cadastro. No formulário, a ação do form html deve ser um POST nos respectivos endpoints já criados em outras tarefas. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
+  </si>
+  <si>
+    <t>Scrum Team e Product Owner</t>
+  </si>
+  <si>
+    <t>Reunião Sprint Review</t>
+  </si>
+  <si>
+    <t>TASK-10</t>
+  </si>
+  <si>
+    <t>Reunião Sprint Retrospective</t>
+  </si>
+  <si>
+    <t>Elaboração do Plano de Projeto, atendendo os critérios do SCRUM e do MPS.BR Nível G.</t>
+  </si>
+  <si>
+    <t>Finalizada</t>
+  </si>
+  <si>
+    <t>Reunião Sprint Planning</t>
+  </si>
+  <si>
+    <t>TASK-11</t>
+  </si>
+  <si>
+    <t>TASK-12</t>
+  </si>
+  <si>
+    <t>Scrum Team</t>
   </si>
 </sst>
 </file>
@@ -829,7 +874,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1075,6 +1120,9 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -34204,8 +34252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34513,10 +34561,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" activeCellId="5" sqref="D8 E8 F8 F9 E9 D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34592,189 +34640,293 @@
       <c r="G5" s="75"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="63" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="64" t="s">
-        <v>97</v>
-      </c>
-      <c r="G6" s="64" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="63"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+    </row>
+    <row r="7" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
         <v>75</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="C7" s="62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="61">
+        <v>42513</v>
+      </c>
+      <c r="E7" s="61">
         <v>42518</v>
       </c>
-      <c r="E7" s="61">
-        <v>42519</v>
-      </c>
-      <c r="F7" s="61"/>
+      <c r="F7" s="61">
+        <v>42518</v>
+      </c>
       <c r="G7" s="62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="65" t="s">
         <v>76</v>
       </c>
       <c r="B8" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="62" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
+        <v>117</v>
+      </c>
+      <c r="C8" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="61">
+        <v>42517</v>
+      </c>
+      <c r="E8" s="61">
+        <v>42517</v>
+      </c>
+      <c r="F8" s="61">
+        <v>42517</v>
+      </c>
       <c r="G8" s="62" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="65" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
+        <v>86</v>
+      </c>
+      <c r="D9" s="61">
+        <v>42519</v>
+      </c>
+      <c r="E9" s="61">
+        <v>42519</v>
+      </c>
       <c r="F9" s="61"/>
       <c r="G9" s="62" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
         <v>78</v>
       </c>
       <c r="B10" s="60" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C10" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
+        <v>86</v>
+      </c>
+      <c r="D10" s="61">
+        <v>42520</v>
+      </c>
+      <c r="E10" s="61">
+        <v>42522</v>
+      </c>
       <c r="F10" s="61"/>
       <c r="G10" s="62" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
         <v>79</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D11" s="61">
-        <v>42509</v>
+        <v>42520</v>
       </c>
       <c r="E11" s="61">
-        <v>42509</v>
+        <v>42523</v>
       </c>
       <c r="F11" s="61"/>
       <c r="G11" s="62" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="65" t="s">
         <v>80</v>
       </c>
       <c r="B12" s="60" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="D12" s="61">
-        <v>42509</v>
+        <v>42520</v>
       </c>
       <c r="E12" s="61">
-        <v>42509</v>
+        <v>42521</v>
       </c>
       <c r="F12" s="61"/>
       <c r="G12" s="62" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="65" t="s">
         <v>81</v>
       </c>
       <c r="B13" s="60" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C13" s="62" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="D13" s="61">
-        <v>42509</v>
+        <v>42522</v>
       </c>
       <c r="E13" s="61">
-        <v>42509</v>
+        <v>42523</v>
       </c>
       <c r="F13" s="61"/>
       <c r="G13" s="62" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="55"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="55"/>
-    </row>
-    <row r="16" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16" s="55"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-    </row>
-    <row r="17" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17" s="55"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-    </row>
-    <row r="18" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18" s="55"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="61">
+        <v>42523</v>
+      </c>
+      <c r="E14" s="61">
+        <v>42524</v>
+      </c>
+      <c r="F14" s="61"/>
+      <c r="G14" s="62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="61">
+        <v>42519</v>
+      </c>
+      <c r="E15" s="61">
+        <v>42524</v>
+      </c>
+      <c r="F15" s="61"/>
+      <c r="G15" s="62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="61">
+        <v>42524</v>
+      </c>
+      <c r="E16" s="61">
+        <v>42524</v>
+      </c>
+      <c r="F16" s="61"/>
+      <c r="G16" s="62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="61">
+        <v>42524</v>
+      </c>
+      <c r="E17" s="61">
+        <v>42524</v>
+      </c>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="65" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="61">
+        <v>42524</v>
+      </c>
+      <c r="E18" s="61">
+        <v>42524</v>
+      </c>
+      <c r="F18" s="61"/>
+      <c r="G18" s="62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="55"/>
+    </row>
+    <row r="20" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20" s="55"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21" s="55"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22" s="55"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>